<commit_message>
Cleaned up and ready for grouping
</commit_message>
<xml_diff>
--- a/Project 1 Plan.xlsx
+++ b/Project 1 Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\07-Project-1\Project_1_Group_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400DD1DD-CFA3-4E53-98A3-83A40BC91089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6198AA-881E-483C-A249-651249E206CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{43CC71D6-9CCC-4F6C-9DB4-27BA6B7779F4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>1a Rating differences between men and women. </t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>https://www.zip-codes.com/city/mo-saint-louis.asp#zipcodes</t>
+  </si>
+  <si>
+    <t>OR find zip_code boundaries and used colored index</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530982F6-EFEC-48D2-B4C6-17DC8279009D}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -861,6 +864,9 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Working but not cleaned up
</commit_message>
<xml_diff>
--- a/Project 1 Plan.xlsx
+++ b/Project 1 Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\07-Project-1\Project_1_Group_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6198AA-881E-483C-A249-651249E206CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7104EC-09DF-4720-ACAC-E4C596172145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{43CC71D6-9CCC-4F6C-9DB4-27BA6B7779F4}"/>
   </bookViews>
@@ -666,7 +666,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>

</xml_diff>